<commit_message>
Updated scenario 4 for password protection
</commit_message>
<xml_diff>
--- a/surendra_testCases.xlsx
+++ b/surendra_testCases.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2193e7a4339f9527/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{573EB1EB-32F7-49C9-98F1-670A2DC81402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD51073C-5A4B-440D-B136-D2B4B26AD4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scenario_1" sheetId="1" r:id="rId1"/>
+    <sheet name="scenario1" sheetId="1" r:id="rId1"/>
     <sheet name="Scenario2" sheetId="2" r:id="rId2"/>
     <sheet name="Scenario3" sheetId="3" r:id="rId3"/>
+    <sheet name="Scenario4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="489">
   <si>
     <t>Email with only a subject and a Body Rendered in DocFusion</t>
   </si>
@@ -1548,12 +1549,521 @@
   <si>
     <t>TestCase_51</t>
   </si>
+  <si>
+    <t>Password Protection where fields are not found in Projections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify Consumer Sends XML Message Successfully</t>
+  </si>
+  <si>
+    <t>TC_API_01</t>
+  </si>
+  <si>
+    <t>This test case verifies that a consumer can send an XML message to the API endpoint and receive the correct response.</t>
+  </si>
+  <si>
+    <t>The API endpoint is up and running.
+The consumer has the necessary authentication credentials (if required).
+The API endpoint URL is known.</t>
+  </si>
+  <si>
+    <t>Prepare the XML message to be sent.
+ Send the XML message to the API endpoint using an HTTP POST request.</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK (or other relevant success code as per API documentation).
+The response body should confirm the successful processing of the XML message.</t>
+  </si>
+  <si>
+    <t>The response headers should include Content-Type: application/xml</t>
+  </si>
+  <si>
+    <t>The XML message has been processed by the API.
+The consumer has received a confirmation response.
+The XML message is sent and processed successfully.
+The response status code is 200 OK.
+The response body contains a success message.
+The response headers include the correct content type.</t>
+  </si>
+  <si>
+    <t>Verify DSMQ Receives XML Message Successfully</t>
+  </si>
+  <si>
+    <t>TC_API_02</t>
+  </si>
+  <si>
+    <t>This test case verifies that the DSMQ can receive an XML message sent by a producer and processes it correctly.</t>
+  </si>
+  <si>
+    <t>DSMQ service is up and running.
+Producer has access to DSMQ endpoint.
+The DSMQ endpoint URL is known.
+Necessary authentication credentials are available if required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The XML message is well-formed and valid according to the DSMQ schema.
+Send the XML message to the DSMQ endpoint using an HTTP POST request.
+</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK (or another relevant success code as per DSMQ documentation).</t>
+  </si>
+  <si>
+    <t>The DSMQ endpoint accepts the request and processes the XML message without errors.
+The response body should confirm the successful reception and processing of the XML message.
+xml
+ Validate the response headers.
+The response headers should include Content-Type: application/xml.
+Check the DSMQ system or logs to ensure the message has been received and processed.
+The DSMQ system should show an entry for the received message with the correct details (MessageID, Timestamp, Customer details).
+The XML message is sent and processed successfully by DSMQ.
+The response status code is 200 OK.
+The response body contains a success message.
+The response headers include the correct content type.
+The DSMQ system logs show the message was received and processed.</t>
+  </si>
+  <si>
+    <t>The XML message has been received and processed by DSMQ.
+The producer has received a confirmation response.</t>
+  </si>
+  <si>
+    <t>Verify Message is Added to Queue Successfully</t>
+  </si>
+  <si>
+    <t>TC_API_03</t>
+  </si>
+  <si>
+    <t>This test case verifies that a message can be successfully added to a queue by sending an XML message to the queue's API endpoint.</t>
+  </si>
+  <si>
+    <t>The queue service is up and running.
+Producer has access to the queue API endpoint.
+The queue API endpoint URL is known.
+Necessary authentication credentials are available if required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepare the XML message to be added to the queue.
+The XML message is well-formed and valid according to the queue schema.
+Send the XML message to the queue API endpoint using an HTTP POST request.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The queue API endpoint accepts the request and processes the XML message without errors.
+The response status code should be 200 OK (or another relevant success code as per API documentation).
+The response body should confirm the successful addition of the message to the queue.</t>
+  </si>
+  <si>
+    <t>The XML message is sent and added to the queue successfully.
+The response status code is 200 OK.
+The response body contains a success message.
+The response headers include the correct content type.
+The queue system logs show the message was added with the correct details</t>
+  </si>
+  <si>
+    <t>The XML message has been added to the queue.
+The producer has received a confirmation response.</t>
+  </si>
+  <si>
+    <t>Verify Enrichment Application Picks Up Message from Queue Successfully</t>
+  </si>
+  <si>
+    <t>TC_API_04</t>
+  </si>
+  <si>
+    <t>This test case verifies that an enrichment application correctly picks up a message from the queue, processes it, and updates the queue status.</t>
+  </si>
+  <si>
+    <t>The queue service is up and running.
+The enrichment application is up and running.
+A valid message is present in the queue.
+Necessary authentication credentials are available if required.</t>
+  </si>
+  <si>
+    <t>At least one message is available in the queue for processing.
+Initiate the enrichment application to pick up messages from the queue.
+Verify that the enrichment application picks up the message from the queue.</t>
+  </si>
+  <si>
+    <t>The message with MessageID 12345 is picked up from the queue by the enrichment application.</t>
+  </si>
+  <si>
+    <t>The message is picked up from the queue by the enrichment application.
+The message is processed and enriched correctly.
+The message status in the queue is updated to indicate successful processing.
+The logs of the enrichment application confirm the processing steps.</t>
+  </si>
+  <si>
+    <t>The message is processed and its status is updated in the queue.
+The enrichment application logs confirm the successful processing of the message.</t>
+  </si>
+  <si>
+    <t>Verify Enrichment Field Exists in Projections</t>
+  </si>
+  <si>
+    <t>TC_API_05</t>
+  </si>
+  <si>
+    <t>This test case verifies that the enrichment field exists in the projections returned by the API after processing a message.</t>
+  </si>
+  <si>
+    <t>The enrichment application is up and running.
+A valid message has been processed by the enrichment application and projections are available.
+Necessary authentication credentials are available if required.
+The API endpoint for retrieving projections is known.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send a request to the API endpoint to retrieve projections.
+Verify the structure of the response body.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if the enrichment field exists in the projections.
+Validate the contents of the enrichment field.
+</t>
+  </si>
+  <si>
+    <t>The response status code is 200 OK.
+The response body contains a list of projections.
+Each projection includes the enrichedData field with the correct enrichment information.</t>
+  </si>
+  <si>
+    <t>The presence of the enrichment field in the projections is confirmed.
+Any issues found are documented for further investigation.</t>
+  </si>
+  <si>
+    <t>Verify Handling of Incomplete Enrichment Process</t>
+  </si>
+  <si>
+    <t>TC_API_06</t>
+  </si>
+  <si>
+    <t>This test case verifies that the API correctly indicates when the enrichment process for a message is not completed.</t>
+  </si>
+  <si>
+    <t>The enrichment application and queue service are up and running.
+A message that has not completed the enrichment process is present in the queue or projections.
+Necessary authentication credentials are available if required.
+The API endpoint for checking the status of enrichment is known.</t>
+  </si>
+  <si>
+    <t>Send a request to the API endpoint to retrieve the status of a specific message.</t>
+  </si>
+  <si>
+    <t>Verify the response status code.
+Verify the structure of the response body
+Validate the handling of incomplete enrichment in the application or system.
+Check the logs of the enrichment application for errors or warnings related to the incomplete process.</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK (or another relevant success code as per API documentation).</t>
+  </si>
+  <si>
+    <t>The status of the message is correctly reported as incomplete.
+Any issues related to the incomplete enrichment process are documented.</t>
+  </si>
+  <si>
+    <t>The response status code is 200 OK.
+The response body indicates that the enrichment process is not completed.
+The status field accurately reflects the incomplete status.
+The details field provides a clear explanation.
+Logs provide information about the cause of the incomplete enrichment process.</t>
+  </si>
+  <si>
+    <t>Verify Enrichment Application Picks Up Non-Enriched XML Message from DSMQ</t>
+  </si>
+  <si>
+    <t>TC_API_07</t>
+  </si>
+  <si>
+    <t>This test case verifies that the enrichment application correctly picks up a non-enriched XML message from DSMQ for processing.</t>
+  </si>
+  <si>
+    <t>The DSMQ service is up and running.
+The enrichment application is up and running.
+A valid non-enriched XML message is present in DSMQ.
+Necessary authentication credentials are available if required.
+The API endpoint for checking the queue or picking up messages is known.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Verify the presence of a non-enriched XML message in DSMQ.
+Initiate the enrichment application to pick up messages from DSMQ.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Document any issues or discrepancies found during the test.</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that the enrichment application picks up the non-enriched XML message from DSMQ.
+Verify the processing of the non-enriched message by the enrichment application.
+Verify the status of the message in DSMQ after processing.</t>
+  </si>
+  <si>
+    <t>The non-enriched XML message is picked up from DSMQ by the enrichment application.
+The message is processed and enriched correctly.
+The message status in DSMQ is updated to indicate successful processing.
+The logs of the enrichment application confirm the processing steps.</t>
+  </si>
+  <si>
+    <t>The non-enriched XML message is picked up and processed by the enrichment application.
+The message status in DSMQ is updated to indicate successful processing.
+Logs provide confirmation of the message processing steps.</t>
+  </si>
+  <si>
+    <t>Verify ACL Converts DSMQ Message for CMA Successfully</t>
+  </si>
+  <si>
+    <t>TC_API_08</t>
+  </si>
+  <si>
+    <t>This test case verifies that the Access Control Layer (ACL) converts a DSMQ message into the appropriate format required by the Central Management Application (CMA).</t>
+  </si>
+  <si>
+    <t>The DSMQ service is up and running.
+The ACL service is up and running.
+The CMA service is up and running.
+A valid message is present in DSMQ that needs to be converted.
+Necessary authentication credentials are available if required.
+The API endpoints for ACL and CMA are known.</t>
+  </si>
+  <si>
+    <t>Verify the presence of a valid DSMQ message.
+Send a request to the ACL endpoint to initiate the conversion process.
+Verify the response status code from the ACL endpoint.
+Verify the structure of the response body.
+Document any issues or discrepancies found during the test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The response status code should be 200 OK (or another relevant success code as per API documentation).
+The converted message should match the format required by CMA.
+</t>
+  </si>
+  <si>
+    <t>The non-enriched XML message is picked up from DSMQ by the ACL.
+The message is converted successfully into the required format by the ACL.
+The converted message is sent to CMA and processed successfully.
+The response status codes from both ACL and CMA are 200 OK.
+The logs of both ACL and CMA confirm the processing steps.</t>
+  </si>
+  <si>
+    <t>The DSMQ message is successfully converted by the ACL and sent to CMA.
+The message is received and processed by CMA.
+Logs provide confirmation of the message conversion and processing steps.</t>
+  </si>
+  <si>
+    <t>Verify Sending Documents Through to DocFusion</t>
+  </si>
+  <si>
+    <t>TC_API_09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This test case verifies that documents are successfully sent through to DocFusion, an external document management system.</t>
+  </si>
+  <si>
+    <t>The system under test is up and running.
+The DocFusion service is up and running.
+Necessary authentication credentials are available if required.
+The API endpoint for sending documents to DocFusion is known.
+A valid document is available to be sent.</t>
+  </si>
+  <si>
+    <t>Prepare the document to be sent to DocFusion.
+Send a request to the DocFusion endpoint to upload the document.
+Verify the response status code from DocFusion.
+Verify the structure of the response body.</t>
+  </si>
+  <si>
+    <t>The response should confirm that the document ID matches the one sent, and the status should indicate success.
+The response status code should be 200 OK (or another relevant success code as per API documentation).</t>
+  </si>
+  <si>
+    <t>The document is successfully sent to and uploaded in DocFusion.
+The response status codes for upload and retrieval are 200 OK.
+The response body confirms successful upload and matches the document ID.
+The retrieved document matches the original document sent.
+The logs confirm the successful handling of the document.</t>
+  </si>
+  <si>
+    <t>The document is successfully sent to DocFusion.
+The document is available in DocFusion and can be retrieved.
+Logs provide confirmation of the document handling steps.</t>
+  </si>
+  <si>
+    <t>Verify Rendering of Body and Attachment in DocFusion</t>
+  </si>
+  <si>
+    <t>TC_API_10</t>
+  </si>
+  <si>
+    <t>This test case verifies that the API correctly renders the body content and attachment within the DocFusion document management system.</t>
+  </si>
+  <si>
+    <t>The system under test is up and running.
+The DocFusion service is up and running.
+Necessary authentication credentials are available if required.
+The API endpoint for uploading and rendering documents in DocFusion is known.
+A valid document with an attachment is available for testing.</t>
+  </si>
+  <si>
+    <t>Prepare the document with body content and attachment to be sent to DocFusion
+Send a request to the DocFusion endpoint to upload the document with body content and attachment.
+Verify the response status code from DocFusion.
+Verify the structure of the response body.</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK (or another relevant success code as per API documentation).
+The converted message should match the format required by CMA.
+Verify the document's presence in DocFusion through a retrieval request.</t>
+  </si>
+  <si>
+    <t>The document with body content and attachment is successfully sent to and uploaded in DocFusion.
+The response status codes for upload and retrieval are 200 OK.
+The response body confirms successful upload and matches the document and attachment IDs.
+The retrieved document and attachment match the original content sent.
+The document and attachment are correctly rendered in the DocFusion UI.
+The logs confirm the successful handling of the document and attachment.</t>
+  </si>
+  <si>
+    <t>The document with body content and attachment is successfully sent to and rendered by DocFusion.
+The document and attachment are available and viewable in DocFusion.
+Logs provide confirmation of the document handling steps.</t>
+  </si>
+  <si>
+    <t>Verify Sending Documentation Through to CMA</t>
+  </si>
+  <si>
+    <t>TC_API_11</t>
+  </si>
+  <si>
+    <t>This test case verifies that the API correctly sends documentation to the Central Management Application (CMA).</t>
+  </si>
+  <si>
+    <t>The system under test is up and running.
+The CMA service is up and running.
+Necessary authentication credentials are available if required.
+The API endpoint for sending documentation to CMA is known.
+A valid document is available for testing.</t>
+  </si>
+  <si>
+    <t>Prepare the document to be sent to CMA.
+Send a request to the CMA endpoint to upload the document.
+Verify the response status code from CMA.
+Verify the structure of the response body.
+Check the logs of the system and CMA for confirmation of document handling.</t>
+  </si>
+  <si>
+    <t>Verify the response status code for the retrieval request.
+The response status code should be 200 OK (or another relevant success code as per API documentation).</t>
+  </si>
+  <si>
+    <t>The document is successfully sent to and uploaded in CMA.
+The response status codes for upload and retrieval are 200 OK.
+The response body confirms successful upload and matches the document ID.
+The retrieved document matches the original document sent.
+The logs confirm the successful handling of the document.</t>
+  </si>
+  <si>
+    <t>The document is successfully sent to CMA.
+The document is available in CMA and can be retrieved.
+Logs provide confirmation of the document handling steps.</t>
+  </si>
+  <si>
+    <t>Verify Determination of Sending Non-Password-Protected Email via Adapter</t>
+  </si>
+  <si>
+    <t>TC_API_12</t>
+  </si>
+  <si>
+    <t>This test case verifies that the API correctly determines whether a non-password-protected email should be sent through the adapter.</t>
+  </si>
+  <si>
+    <t>The system under test is up and running.
+The adapter service is up and running.
+Necessary authentication credentials are available if required.
+The API endpoint for email determination is known.
+Sample emails (both password-protected and non-password-protected) are available for testing.</t>
+  </si>
+  <si>
+    <t>Prepare the non-password-protected email payload.
+Send a request to the API endpoint to determine if the email should be sent via the adapter.
+Send a request to the API endpoint to determine if the password-protected email should be sent via the adapter.
+Verify the response status code from the API for the password-protected email.</t>
+  </si>
+  <si>
+    <t>The response status codes for both requests are 200 OK.
+The response body correctly indicates whether the email should be sent via the adapter based on its password protection status.
+The logs confirm the correct handling of the emails based on the determination.</t>
+  </si>
+  <si>
+    <t>The determination process correctly identifies whether the email should be sent via the adapter.
+The system and adapter logs provide confirmation of email handling steps.</t>
+  </si>
+  <si>
+    <t>Verify Sending Status Updates from CMA to DSMQ</t>
+  </si>
+  <si>
+    <t>TC_API_13</t>
+  </si>
+  <si>
+    <t>This test case verifies that the Central Management Application (CMA) correctly sends status updates to the Distributed Systems Message Queue (DSMQ) via the API.</t>
+  </si>
+  <si>
+    <t>The Central Management Application (CMA) is up and running.
+The Distributed Systems Message Queue (DSMQ) is up and running.
+Necessary authentication credentials are available if required.
+The API endpoint for sending status updates from CMA to DSMQ is known.
+A valid status update message is available for testing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepare the status update message to be sent from CMA to DSMQ.
+Send a request from CMA to the API endpoint to send the status update message to DSMQ.
+Verify the response status code from the API.
+Verify the structure of the response body.
+Validate the contents of the response.
+Check the logs of CMA and DSMQ for confirmation of status update message handling.
+Document any issues or discrepancies found during the test.
+</t>
+  </si>
+  <si>
+    <t>The response status code for the request is 200 OK.</t>
+  </si>
+  <si>
+    <t>The response body confirms successful submission of the status update message.
+The logs confirm the correct handling of the status update message by both CMA and DSMQ.</t>
+  </si>
+  <si>
+    <t>The status update message is successfully sent from CMA to DSMQ.
+Logs provide confirmation of the status update message handling steps.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1579,8 +2089,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1603,6 +2125,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1698,7 +2226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1720,15 +2248,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1740,6 +2259,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2024,8 +2564,8 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="88" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="E12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:J13"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2045,20 +2585,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
@@ -2462,7 +3002,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="58" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
@@ -2478,20 +3018,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -2817,1302 +3357,1716 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E34D38-4229-4676-BE70-E5B405438767}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C5"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="34.85546875" style="12"/>
-    <col min="6" max="6" width="14.28515625" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="34.85546875" style="12"/>
+    <col min="1" max="5" width="34.85546875" style="9"/>
+    <col min="6" max="6" width="14.28515625" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="34.85546875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" ht="30.75">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="106.5">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" ht="91.5">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" ht="106.5">
+      <c r="A5" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" ht="91.5">
+      <c r="A6" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" ht="91.5">
+      <c r="A7" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="76.5">
+      <c r="A8" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="121.5">
+      <c r="A9" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" ht="106.5">
+      <c r="A10" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" ht="106.5">
+      <c r="A11" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="106.5">
+      <c r="A12" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="106.5">
+      <c r="A13" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" ht="60.75">
+      <c r="A14" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="60.75">
+      <c r="A15" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" ht="60.75">
+      <c r="A16" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" ht="60.75">
+      <c r="A17" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="60.75">
+      <c r="A18" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" ht="60.75">
+      <c r="A19" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="1:10" ht="60.75">
+      <c r="A20" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="1:10" ht="60.75">
+      <c r="A21" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:10" ht="76.5">
+      <c r="A22" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="1:10" ht="76.5">
+      <c r="A23" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="1:10" ht="76.5">
+      <c r="A24" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="1:10" ht="91.5">
+      <c r="A25" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="1:10" ht="106.5">
+      <c r="A26" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="1:10" ht="91.5">
+      <c r="A27" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="1:10" ht="60.75">
+      <c r="A28" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="1:10" ht="91.5">
+      <c r="A29" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="1:10" ht="76.5">
+      <c r="A30" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="1:10" ht="76.5">
+      <c r="A31" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="1:10" ht="76.5">
+      <c r="A32" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+    </row>
+    <row r="33" spans="1:10" ht="60.75">
+      <c r="A33" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="1:10" ht="76.5">
+      <c r="A34" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+    </row>
+    <row r="35" spans="1:10" ht="60.75">
+      <c r="A35" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+    </row>
+    <row r="36" spans="1:10" ht="60.75">
+      <c r="A36" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+    </row>
+    <row r="37" spans="1:10" ht="60.75">
+      <c r="A37" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+    </row>
+    <row r="38" spans="1:10" ht="76.5">
+      <c r="A38" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+    </row>
+    <row r="39" spans="1:10" ht="409.6">
+      <c r="A39" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="91.5">
+      <c r="A40" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+    </row>
+    <row r="41" spans="1:10" ht="91.5">
+      <c r="A41" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+    </row>
+    <row r="42" spans="1:10" ht="121.5">
+      <c r="A42" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+    </row>
+    <row r="43" spans="1:10" ht="76.5">
+      <c r="A43" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+    </row>
+    <row r="44" spans="1:10" ht="91.5">
+      <c r="A44" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+    </row>
+    <row r="45" spans="1:10" ht="91.5">
+      <c r="A45" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+    </row>
+    <row r="46" spans="1:10" ht="106.5">
+      <c r="A46" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+    </row>
+    <row r="47" spans="1:10" ht="91.5">
+      <c r="A47" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+    </row>
+    <row r="48" spans="1:10" ht="106.5">
+      <c r="A48" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+    </row>
+    <row r="49" spans="1:10" ht="91.5">
+      <c r="A49" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+    </row>
+    <row r="50" spans="1:10" ht="121.5">
+      <c r="A50" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+    </row>
+    <row r="51" spans="1:10" ht="106.5">
+      <c r="A51" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+    </row>
+    <row r="52" spans="1:10" ht="106.5">
+      <c r="A52" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+    </row>
+    <row r="53" spans="1:10" ht="409.6">
+      <c r="A53" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04436822-DFE4-4252-A5DC-3AA8D26C5943}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="46.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="46.140625" style="9"/>
+    <col min="2" max="2" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="46.140625" style="9"/>
+    <col min="10" max="10" width="6.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="46.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="137.25">
+      <c r="A3" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="351">
+      <c r="A4" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>400</v>
+      </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" ht="106.5">
-      <c r="A5" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" ht="91.5">
-      <c r="A6" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" ht="91.5">
-      <c r="A7" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" ht="76.5">
-      <c r="A8" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+    </row>
+    <row r="5" spans="1:10" ht="121.5">
+      <c r="A5" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="106.5">
+      <c r="A6" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="121.5">
+      <c r="A7" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="121.5">
+      <c r="A8" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="121.5">
-      <c r="A9" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" ht="106.5">
-      <c r="A10" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" ht="106.5">
-      <c r="A11" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" ht="106.5">
-      <c r="A12" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" ht="106.5">
-      <c r="A13" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" ht="60.75">
-      <c r="A14" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" ht="60.75">
-      <c r="A15" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="1:10" ht="60.75">
-      <c r="A16" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" ht="60.75">
-      <c r="A17" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-    </row>
-    <row r="18" spans="1:10" ht="60.75">
-      <c r="A18" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="1:10" ht="60.75">
-      <c r="A19" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-    </row>
-    <row r="20" spans="1:10" ht="60.75">
-      <c r="A20" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="1:10" ht="60.75">
-      <c r="A21" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="1:10" ht="76.5">
-      <c r="A22" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="1:10" ht="76.5">
-      <c r="A23" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-    </row>
-    <row r="24" spans="1:10" ht="76.5">
-      <c r="A24" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-    </row>
-    <row r="25" spans="1:10" ht="91.5">
-      <c r="A25" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-    </row>
-    <row r="26" spans="1:10" ht="106.5">
-      <c r="A26" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-    </row>
-    <row r="27" spans="1:10" ht="91.5">
-      <c r="A27" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-    </row>
-    <row r="28" spans="1:10" ht="60.75">
-      <c r="A28" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-    </row>
-    <row r="29" spans="1:10" ht="91.5">
-      <c r="A29" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-    </row>
-    <row r="30" spans="1:10" ht="76.5">
-      <c r="A30" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-    </row>
-    <row r="31" spans="1:10" ht="76.5">
-      <c r="A31" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="1:10" ht="76.5">
-      <c r="A32" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-    </row>
-    <row r="33" spans="1:10" ht="60.75">
-      <c r="A33" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-    </row>
-    <row r="34" spans="1:10" ht="76.5">
-      <c r="A34" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-    </row>
-    <row r="35" spans="1:10" ht="60.75">
-      <c r="A35" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36" spans="1:10" ht="60.75">
-      <c r="A36" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>309</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-    </row>
-    <row r="37" spans="1:10" ht="60.75">
-      <c r="A37" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-    </row>
-    <row r="38" spans="1:10" ht="76.5">
-      <c r="A38" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13" t="s">
-        <v>321</v>
-      </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-    </row>
-    <row r="39" spans="1:10" ht="409.6">
-      <c r="A39" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>322</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="J39" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="91.5">
-      <c r="A40" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>324</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-    </row>
-    <row r="41" spans="1:10" ht="91.5">
-      <c r="A41" s="13" t="s">
-        <v>328</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>328</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-    </row>
-    <row r="42" spans="1:10" ht="121.5">
-      <c r="A42" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-    </row>
-    <row r="43" spans="1:10" ht="76.5">
-      <c r="A43" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>337</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
-    </row>
-    <row r="44" spans="1:10" ht="91.5">
-      <c r="A44" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-    </row>
-    <row r="45" spans="1:10" ht="91.5">
-      <c r="A45" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13" t="s">
-        <v>350</v>
-      </c>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-    </row>
-    <row r="46" spans="1:10" ht="106.5">
-      <c r="A46" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-    </row>
-    <row r="47" spans="1:10" ht="91.5">
-      <c r="A47" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13" t="s">
-        <v>360</v>
-      </c>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-    </row>
-    <row r="48" spans="1:10" ht="106.5">
-      <c r="A48" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-    </row>
-    <row r="49" spans="1:10" ht="91.5">
-      <c r="A49" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-    </row>
-    <row r="50" spans="1:10" ht="121.5">
-      <c r="A50" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-    </row>
-    <row r="51" spans="1:10" ht="106.5">
-      <c r="A51" s="13" t="s">
-        <v>374</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>374</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-    </row>
-    <row r="52" spans="1:10" ht="106.5">
-      <c r="A52" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-    </row>
-    <row r="53" spans="1:10" ht="409.6">
-      <c r="A53" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="J53" s="14" t="s">
-        <v>119</v>
+      <c r="A9" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>439</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="152.25">
+      <c r="A10" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="152.25">
+      <c r="A11" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="183">
+      <c r="A12" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="152.25">
+      <c r="A13" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="121.5">
+      <c r="A14" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>477</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="183">
+      <c r="A15" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uploaded few test for scenario 5
</commit_message>
<xml_diff>
--- a/surendra_testCases.xlsx
+++ b/surendra_testCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHILIPS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC2B082-2227-4F1E-A64F-9D195CADC4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B9482D-241A-4ABF-A330-4CC272F262CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="502">
   <si>
     <t>Email with only a subject and a Body Rendered in DocFusion</t>
   </si>
@@ -629,18 +629,6 @@
     <t>Access to the API endpoint.
 Valid credentials (if authentication is required).
 A tool to send HTTP requests, such as Postman or Curl.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ensure you have the necessary access credentials for the API.
-Open your preferred HTTP request tool Postman 
-Prepare the XML message to be sent
-Set the request method to POST.
-Set the request URL to the API endpoint: 
-In the headers, set Content-Type to application/xml.
-If authentication is required, add the appropriate authentication headers 
-In the request body, paste the XML message defined in step 3.
-Send the request.
-</t>
   </si>
   <si>
     <t>Check the status code of the response. It should be 200 OK or another successful status code as per API documentation.
@@ -2051,12 +2039,84 @@
   <si>
     <t>Password Protection with Information Existing in Projection</t>
   </si>
+  <si>
+    <t xml:space="preserve">Ensure you have the necessary access credentials for the API.
+Open your preferred HTTP request tool Postman 
+Prepare the XML message to be sent
+Set the request method to POST.
+Set the request URL to the API endpoint: 
+In the headers, set Content-Type to application/xml.
+If authentication is required, add the appropriate authentication headers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure you have the necessary access credentials for the API.
+Open your preferred HTTP request tool Postman 
+Prepare the XML message to be sent
+Set the request method to POST.
+Set the request URL to the API endpoint: 
+In the headers, set Content-Type to application/xml.
+If authentication is required, add the appropriate authentication headers 
+</t>
+  </si>
+  <si>
+    <t>Test_001</t>
+  </si>
+  <si>
+    <t>Test_002</t>
+  </si>
+  <si>
+    <t>Test_003</t>
+  </si>
+  <si>
+    <t>To ensure the enrichment application correctly picks up and processes messages from the queue.</t>
+  </si>
+  <si>
+    <t>The message queue service is up and running.
+The enrichment application is deployed and connected to the message queue.
+Test messages are available in the queue.</t>
+  </si>
+  <si>
+    <t>Test_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert Test Message into Queue
+Action: Use a message queue client or API to insert the sample message into the test-queue.
+Expected Result: The message should be successfully inserted into the queueTrigger Enrichment Application
+Action: Ensure the enrichment application is running and monitoring the queue.
+Expected Result: The application should be in a ready state to pick up messages from the queue.
+Verify Message Picked Up
+Action: Check the logs or monitoring tool of the enrichment application to verify that the message with id: 12345 is picked up from the queue.
+Expected Result: The logs should indicate that the message is picked up for processing
+Validate Message Processing
+Action: Check the output or the destination where the enriched message is stored (e.g., another queue, database, or log).
+Expected Result: The processed message should match the expected processed message format, indicating it was enriched and a timestamp was added.
+</t>
+  </si>
+  <si>
+    <t>The message is successfully inserted into the test-queue.
+The enrichment application picks up the message from the queue.
+The message is processed and enriched correctly.
+No errors occur during the process.
+Test data is cleaned up after the test.</t>
+  </si>
+  <si>
+    <t>The message queue and the enrichment application return to their normal state.
+Any test data inserted into the queue or produced by the enrichment application is removed.</t>
+  </si>
+  <si>
+    <t>Check the status code of the response</t>
+  </si>
+  <si>
+    <t>Ensure the time format in the processed message's timestamp matches the expected ISO 8601 format.
+If the enrichment application has a retry mechanism, verify that the message is processed only once.
+This test assumes synchronous message processing. Adjust the verification steps if the application processes messages asynchronously.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2093,6 +2153,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2219,7 +2285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2274,6 +2340,25 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2556,10 +2641,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="88" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2994,10 +3079,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03E9891-F9C2-4E9A-9FC1-C5F5A86348EB}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="58" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="58" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3072,51 +3157,51 @@
         <v>124</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="288.60000000000002" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
@@ -3124,7 +3209,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>42</v>
@@ -3156,7 +3241,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>52</v>
@@ -3188,7 +3273,7 @@
         <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>72</v>
@@ -3217,60 +3302,60 @@
     </row>
     <row r="8" spans="1:12" ht="202.2" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -3278,7 +3363,7 @@
         <v>100</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>102</v>
@@ -3310,7 +3395,7 @@
         <v>110</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>112</v>
@@ -3364,7 +3449,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -3410,23 +3495,23 @@
     </row>
     <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>163</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>164</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -3434,23 +3519,23 @@
     </row>
     <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>168</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>169</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -3458,23 +3543,23 @@
     </row>
     <row r="5" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
@@ -3482,23 +3567,23 @@
     </row>
     <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>178</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -3506,23 +3591,23 @@
     </row>
     <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -3530,23 +3615,23 @@
     </row>
     <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -3554,23 +3639,23 @@
     </row>
     <row r="9" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>192</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -3578,23 +3663,23 @@
     </row>
     <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>195</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>196</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -3602,23 +3687,23 @@
     </row>
     <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -3626,23 +3711,23 @@
     </row>
     <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -3650,23 +3735,23 @@
     </row>
     <row r="13" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>208</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -3674,23 +3759,23 @@
     </row>
     <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>213</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -3698,23 +3783,23 @@
     </row>
     <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>216</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -3722,23 +3807,23 @@
     </row>
     <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>220</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -3746,23 +3831,23 @@
     </row>
     <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>225</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -3770,23 +3855,23 @@
     </row>
     <row r="18" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="C18" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>228</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>229</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -3794,23 +3879,23 @@
     </row>
     <row r="19" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>233</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>234</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -3818,23 +3903,23 @@
     </row>
     <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="C20" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -3842,23 +3927,23 @@
     </row>
     <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C21" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>241</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>242</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -3866,23 +3951,23 @@
     </row>
     <row r="22" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>246</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>247</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
@@ -3890,23 +3975,23 @@
     </row>
     <row r="23" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="E23" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>252</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
@@ -3914,23 +3999,23 @@
     </row>
     <row r="24" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>255</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -3938,23 +4023,23 @@
     </row>
     <row r="25" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>260</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
@@ -3962,23 +4047,23 @@
     </row>
     <row r="26" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>263</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
@@ -3986,23 +4071,23 @@
     </row>
     <row r="27" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>269</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>270</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
@@ -4010,23 +4095,23 @@
     </row>
     <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="C28" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>274</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>275</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -4034,23 +4119,23 @@
     </row>
     <row r="29" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="C29" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>279</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>280</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
@@ -4058,23 +4143,23 @@
     </row>
     <row r="30" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>284</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>285</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
@@ -4082,23 +4167,23 @@
     </row>
     <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="C31" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
@@ -4106,23 +4191,23 @@
     </row>
     <row r="32" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>293</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>294</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
@@ -4130,23 +4215,23 @@
     </row>
     <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="C33" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>297</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>298</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
@@ -4154,23 +4239,23 @@
     </row>
     <row r="34" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="C34" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>301</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>302</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
@@ -4178,23 +4263,23 @@
     </row>
     <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>305</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>306</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
@@ -4202,23 +4287,23 @@
     </row>
     <row r="36" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="C36" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>309</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>310</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
@@ -4226,23 +4311,23 @@
     </row>
     <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="C37" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="D37" s="10" t="s">
+      <c r="E37" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>315</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
@@ -4250,23 +4335,23 @@
     </row>
     <row r="38" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="C38" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>319</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>320</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
@@ -4277,7 +4362,7 @@
         <v>80</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>82</v>
@@ -4306,23 +4391,23 @@
     </row>
     <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="C40" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>325</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>326</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
@@ -4330,23 +4415,23 @@
     </row>
     <row r="41" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="C41" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="E41" s="10" t="s">
         <v>329</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>330</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
@@ -4354,23 +4439,23 @@
     </row>
     <row r="42" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="C42" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>333</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>334</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
@@ -4378,23 +4463,23 @@
     </row>
     <row r="43" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="C43" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="D43" s="10" t="s">
+      <c r="E43" s="10" t="s">
         <v>338</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>339</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
@@ -4402,23 +4487,23 @@
     </row>
     <row r="44" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="C44" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>343</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>344</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
@@ -4426,23 +4511,23 @@
     </row>
     <row r="45" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="C45" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="D45" s="10" t="s">
+      <c r="E45" s="10" t="s">
         <v>348</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>349</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
@@ -4450,23 +4535,23 @@
     </row>
     <row r="46" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="C46" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D46" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="C46" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="D46" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>353</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>354</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
@@ -4474,23 +4559,23 @@
     </row>
     <row r="47" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="C47" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="D47" s="10" t="s">
+      <c r="E47" s="10" t="s">
         <v>358</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>359</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
@@ -4498,23 +4583,23 @@
     </row>
     <row r="48" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="C48" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>362</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>363</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
@@ -4522,23 +4607,23 @@
     </row>
     <row r="49" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="C49" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="D49" s="10" t="s">
+      <c r="E49" s="10" t="s">
         <v>367</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>368</v>
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
@@ -4546,23 +4631,23 @@
     </row>
     <row r="50" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="C50" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="D50" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="10" t="s">
         <v>372</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>373</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
@@ -4570,23 +4655,23 @@
     </row>
     <row r="51" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="C51" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="D51" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="D51" s="10" t="s">
+      <c r="E51" s="10" t="s">
         <v>376</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>377</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
@@ -4594,23 +4679,23 @@
     </row>
     <row r="52" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>378</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="C52" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="D52" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="D52" s="10" t="s">
+      <c r="E52" s="10" t="s">
         <v>380</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>381</v>
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
@@ -4621,7 +4706,7 @@
         <v>110</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>112</v>
@@ -4676,7 +4761,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -4722,344 +4807,344 @@
     </row>
     <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>387</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>389</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>391</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="14" t="s">
         <v>394</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>399</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>400</v>
       </c>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>407</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>415</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>423</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>432</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="15" t="s">
         <v>437</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F9" s="16" t="s">
         <v>438</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="G9" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>440</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>446</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>448</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>456</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>460</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>464</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>472</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>479</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>482</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>486</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>487</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -5072,17 +5157,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2630F56D-01BC-468E-A632-55FBB048E4ED}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="47.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -5094,7 +5180,7 @@
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
     </row>
-    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -5126,10 +5212,158 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:10" s="23" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>491</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="20" customFormat="1" ht="245.4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="20" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="25" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>500</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated scenarion 5 with pending test cases
</commit_message>
<xml_diff>
--- a/surendra_testCases.xlsx
+++ b/surendra_testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHILIPS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B9482D-241A-4ABF-A330-4CC272F262CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED24F8E-B629-41F1-A82A-0BCBA6FEF900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="590">
   <si>
     <t>Email with only a subject and a Body Rendered in DocFusion</t>
   </si>
@@ -2110,6 +2110,462 @@
     <t>Ensure the time format in the processed message's timestamp matches the expected ISO 8601 format.
 If the enrichment application has a retry mechanism, verify that the message is processed only once.
 This test assumes synchronous message processing. Adjust the verification steps if the application processes messages asynchronously.</t>
+  </si>
+  <si>
+    <t>Verify the existence of the enrichment field in the projections endpoint response.</t>
+  </si>
+  <si>
+    <t>Test_005</t>
+  </si>
+  <si>
+    <t>Test_006</t>
+  </si>
+  <si>
+    <t>Test_007</t>
+  </si>
+  <si>
+    <t>To ensure that the 'enrichment' field is present in the response of the projections endpoint.</t>
+  </si>
+  <si>
+    <t>The API server is up and running.
+Valid authentication token (if required).
+Access to the API documentation to understand the structure and endpoint of the projections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send a GET request to the projections endpoint
+</t>
+  </si>
+  <si>
+    <t>Check the status code of the response. It should be 200 OK.
+Parse the JSON response body.
+Verify that the 'enrichment' field exists in the response.</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK.
+The JSON response should include an 'enrichment' field.</t>
+  </si>
+  <si>
+    <t>If the 'enrichment' field is missing, log a defect with the details of the request and response for further investigation.</t>
+  </si>
+  <si>
+    <t>Verify the completeness of the enrichment field in the projections endpoint response.</t>
+  </si>
+  <si>
+    <t>To ensure that the 'enrichment' field in the response of the projections endpoint is complete and contains all expected subfields.</t>
+  </si>
+  <si>
+    <t>The API server is up and running.
+Valid authentication token (if required).
+Access to the API documentation to understand the expected structure of the 'enrichment' field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure the API server is running.
+Have the authentication token ready (if required).
+Send a GET request to the projections endpoint.
+</t>
+  </si>
+  <si>
+    <t>Check the status code of the response. It should be 200 OK.
+Parse the JSON response body.
+Verify that the 'enrichment' field exists in each projection object.
+Check that the 'enrichment' field contains all expected subfields (field1, field2, field3)</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK.
+Each 'enrichment' field in the projection objects should contain the subfields field1, field2, and field3.</t>
+  </si>
+  <si>
+    <t>Status code is 200.
+ Each 'enrichment' field is present and complete with subfields field1, field2, and field3.</t>
+  </si>
+  <si>
+    <t>If any subfield is missing or the 'enrichment' field itself is missing, log a defect with the details of the request and response for further investigation.</t>
+  </si>
+  <si>
+    <t>Verify that a message received from the enrichment process is correctly written to the queue.</t>
+  </si>
+  <si>
+    <t>To ensure that the system correctly receives a message from the enrichment process and successfully writes this message to the queue.</t>
+  </si>
+  <si>
+    <t>The API server and the message queue server are up and running.
+Valid authentication token (if required).
+Access to the API documentation to understand the message format.
+Tools for inspecting the queue, such as a message queue client (e.g., RabbitMQ management interface, AWS SQS console).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparation:
+Ensure the API and message queue servers are running.
+Have the authentication token ready (if required).
+Prepare a sample message to send to the enrichment endpoint.
+Send Message to Enrichment:
+Send a POST request with the sample message to the enrichment endpoint
+</t>
+  </si>
+  <si>
+    <t>Check the status code of the response. It should be 200 OK or another appropriate success status code.</t>
+  </si>
+  <si>
+    <t>The response status code from the enrichment endpoint should be 200 OK.
+The message queue enrichmentQueue should contain the message with the correct content.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Status code is 200.
+ The message is present in the enrichmentQueue.
+ The message content in the queue matches the sample message.</t>
+  </si>
+  <si>
+    <t>If the message is not present in the queue or if the content does not match, log a defect with the details of the request, response, and queue inspection for further investigation.</t>
+  </si>
+  <si>
+    <t>Verify that ACL correctly translates the message received from DSMQ</t>
+  </si>
+  <si>
+    <t>Test_008</t>
+  </si>
+  <si>
+    <t>Test_009</t>
+  </si>
+  <si>
+    <t>To ensure that the ACL system correctly translates a message received from the DSMQ queue and outputs the expected translated message.</t>
+  </si>
+  <si>
+    <t>The API server and the DSMQ message queue server are up and running.
+ACL translation service is up and running.
+Access to the API documentation to understand the message format.
+Tools for inspecting the DSMQ queue, such as a message queue client (RabbitMQ management interface, AWS SQS console).
+Knowledge of the expected translation rules or output.</t>
+  </si>
+  <si>
+    <t>Preparation:
+Ensure the API server, DSMQ server, and ACL translation service are running.
+Use the message queue client to place a sample message into the dsmqQueue.
+Place the sample message into the dsmqQueue
+Process Message:
+Wait for the ACL system to process the message from dsmqQueue and place the translated message into the translatedQueue.
+Inspect Translated Queue:
+Use the message queue client to inspect the translatedQueue.
+Verify that the translated message is present in the queue.
+Ensure that the translated message content matches the expected translated message.</t>
+  </si>
+  <si>
+    <t>The translated message should be present in the translatedQueue.
+The message content should match the expected translated message</t>
+  </si>
+  <si>
+    <t>Verify that the translated message is present in the queue.</t>
+  </si>
+  <si>
+    <t>If the translated message is not present in the queue or if the content does not match, log a defect with the details of the DSMQ queue message, translated queue message, and any relevant logs for further investigation.</t>
+  </si>
+  <si>
+    <t>SMQ Queue name: dsmqQueue
+Translated Queue name: translatedQueue</t>
+  </si>
+  <si>
+    <t>Verify sending a document through to DocFusion and receiving the expected response.</t>
+  </si>
+  <si>
+    <t>To ensure that the system correctly sends a document to the DocFusion endpoint and receives the expected response indicating successful processing.</t>
+  </si>
+  <si>
+    <t>The API server and the DocFusion service are up and running.
+Valid authentication token (if required).
+Access to the API documentation to understand the document format and endpoint.
+A sample document ready for testing.</t>
+  </si>
+  <si>
+    <t>Preparation:
+Ensure the API server and DocFusion service are running.
+Have the authentication token ready (if required).
+Prepare the sample document for sending.</t>
+  </si>
+  <si>
+    <t>Method: POST
+Authentication: Bearer Token (if applicable)</t>
+  </si>
+  <si>
+    <t>Check the status code of the response. It should be 200 OK or another appropriate success status code.
+Parse the JSON response body.
+Verify that the response contains the expected status, message, and document URL.</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK.
+The JSON response should include:
+status field with value "success".
+message field with value "Document processed successfully."
+documentUrl field with a valid URL to the processed document.</t>
+  </si>
+  <si>
+    <t>Status code is 200.
+ Response contains status field with value "success".
+ Response contains message field with value "Document processed successfully."
+ Response contains documentUrl field with a valid URL.</t>
+  </si>
+  <si>
+    <t>Verify that DocFusion correctly renders the body and attachment from the provided input</t>
+  </si>
+  <si>
+    <t>Test_010</t>
+  </si>
+  <si>
+    <t>Test_011</t>
+  </si>
+  <si>
+    <t>Test_012</t>
+  </si>
+  <si>
+    <t>To ensure that the system correctly sends a request with both body content and an attachment to the DocFusion endpoint and receives the expected response indicating successful processing.</t>
+  </si>
+  <si>
+    <t>The API server and DocFusion service are up and running.
+Valid authentication token (if required).
+Access to the API documentation to understand the document and attachment format and endpoint.
+A sample document and attachment file ready for testing.</t>
+  </si>
+  <si>
+    <t>Preparation:
+Ensure the API server and DocFusion service are running.
+Have the authentication token ready (if required).
+Prepare the sample JSON body and attachment file (report.pdf).
+Send a POST request with the sample JSON body and attachment file to the DocFusion endpoint using a tool like curl or Postman.</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK.
+The JSON response should include:
+status field with value "success".
+message field with value "Document and attachment processed successfully."
+documentUrl field with a valid URL to the processed document.</t>
+  </si>
+  <si>
+    <t>Status code is 200.
+ Response contains status field with value "success".
+ Response contains message field with value "Document and attachment processed successfully."
+ Response contains documentUrl field with a valid URL.</t>
+  </si>
+  <si>
+    <t>If the response status is not 200 or if the expected fields are missing, log a defect with the details of the request and response for further investigation.</t>
+  </si>
+  <si>
+    <t>Verify that the system sends documentation to the CMA endpoint and receives the expected response.</t>
+  </si>
+  <si>
+    <t>To ensure that the system correctly sends documentation to the CMA (Content Management Application) endpoint and receives the expected response indicating successful processing.</t>
+  </si>
+  <si>
+    <t>The API server and the CMA service are up and running.
+Valid authentication token (if required).
+Access to the API documentation to understand the document format and endpoint.
+A sample document ready for testing.</t>
+  </si>
+  <si>
+    <t>Preparation:
+Ensure the API server and CMA service are running.
+Have the authentication token ready (if required).
+Prepare the sample document for sending.</t>
+  </si>
+  <si>
+    <t>The response status code should be 200 OK.
+The JSON response should include:
+status field with value "success".
+message field with value "Documentation processed successfully."
+documentUrl field with a valid URL to the processed document.</t>
+  </si>
+  <si>
+    <t>Status code is 200.
+ Response contains status field with value "success".
+ Response contains message field with value "Documentation processed successfully."
+ Response contains documentUrl field with a valid URL.</t>
+  </si>
+  <si>
+    <t>Verify that the system passes rendered documents to the Password Protection Application and receives the expected response.</t>
+  </si>
+  <si>
+    <t>Ensure that the password protection application successfully applies a password to rendered documents and that the password works correctly.</t>
+  </si>
+  <si>
+    <t>Password protection application installed and configured.
+Rendered document (e.g., PDF, DOCX) available for testing.
+Known password for testing (e.g., "Test@123").</t>
+  </si>
+  <si>
+    <t>Step Description: Launch the password protection application.
+Expected Result: Application opens without any errors and is ready to use.
+Select Document
+Step Description: Navigate to the option to select a document for password protection.
+Expected Result: The application allows the user to browse and select a document from the file system.
+Upload Document
+Step Description: Select and upload the rendered document for password protection.
+Expected Result: The document is successfully uploaded and displayed in the application.
+Set Password
+Step Description: Enter the password (e.g., "Test@123") in the designated field and confirm the password.
+Expected Result: The application accepts the password and shows a confirmation message.
+Apply Password Protection
+Step Description: Click on the button to apply the password protection to the document.
+Expected Result: The application processes the document and applies the password protection. A confirmation message indicating successful password protection should be displayed.
+Download Protected Document
+Step Description: Download the password-protected document from the application.
+Expected Result: The document is successfully downloaded and saved to the local file system.</t>
+  </si>
+  <si>
+    <t>Step Description: Attempt to open the downloaded document using a compatible viewer.
+Expected Result: The viewer prompts for a password before opening the document.</t>
+  </si>
+  <si>
+    <t>The rendered document should remain password-protected.
+The application should log the password protection process (if applicable).</t>
+  </si>
+  <si>
+    <t>Ensure to use a strong password and avoid common or easily guessable passwords.
+Check for any application-specific logging or auditing features that might record the password protection process for later review.</t>
+  </si>
+  <si>
+    <t>Verify Complete Password Protection Functionality via API</t>
+  </si>
+  <si>
+    <t>Test_013</t>
+  </si>
+  <si>
+    <t>Test_014</t>
+  </si>
+  <si>
+    <t>Test_015</t>
+  </si>
+  <si>
+    <t>Ensure that the API successfully applies password protection to documents and handles various scenarios related to password protection.</t>
+  </si>
+  <si>
+    <t>Access to the API under test.
+Rendered documents available for testing.
+Testing environment set up and configured.</t>
+  </si>
+  <si>
+    <t>Authenticate with API
+Step Description: Authenticate with the API using valid credentials (e.g., API key, OAuth token).
+Expected Result: Successful authentication response with a valid token or session established.
+Select Document
+Step Description: Choose a rendered document to apply password protection.
+Expected Result: The API accepts the document selection request and acknowledges the document to be protected.
+Set Password
+Step Description: Send a request to set a password for the selected document.
+Expected Result: The API accepts the password and confirms its successful assignment to the document.
+Apply Password Protection
+Step Description: Trigger the API to apply password protection to the document using the provided password.
+Expected Result: The API processes the document and returns a success response indicating that password protection has been applied.
+Retrieve Protected Document
+Step Description: Retrieve the protected document using the API.
+Expected Result: The API provides a link or a downloadable resource for the protected document.
+Attempt to Open Document without Password
+Step Description: Try to open the protected document without providing any password.
+Expected Result: Access to the document should be denied, and an error indicating the need for a password should be returned.
+Attempt to Open Document with Incorrect Password
+Step Description: Try to open the protected document with an incorrect password.
+Expected Result: Access to the document should be denied, and an error indicating an incorrect password should be returned.
+Open Document with Correct Password
+Step Description: Open the protected document using the correct password.
+Expected Result: Access to the document should be granted, and the document contents should be visible and intact.
+Check Document Integrity
+Step Description: Verify that the protected document's contents are intact and have not been altered during password protection.
+Expected Result: The document contents should match the original document before password protection.</t>
+  </si>
+  <si>
+    <t>The document should remain password-protected until the password protection is removed or updated via the API.
+Any error or exception messages should be logged for troubleshooting purposes.</t>
+  </si>
+  <si>
+    <t>Ensure that the API responses include appropriate error messages for different scenarios (e.g., incorrect password, invalid document).
+Perform boundary testing with different lengths and types of passwords to ensure robustness.
+Test the API's performance under varying document sizes to ensure scalability.</t>
+  </si>
+  <si>
+    <t>Verify Sending Password-Protected Document to Client via Adapter</t>
+  </si>
+  <si>
+    <t>Ensure that the API, along with the adapter, successfully sends password-protected documents to clients and that clients can access them securely.</t>
+  </si>
+  <si>
+    <t>Access to the API under test.
+Adapter configured to communicate with the API and clients.
+Rendered documents available for testing.
+Client application or system set up to receive documents via the adapter.</t>
+  </si>
+  <si>
+    <t>Authenticate with API
+Step Description: Authenticate with the API using valid credentials (e.g., API key, OAuth token).
+Expected Result: Successful authentication response with a valid token or session established.
+Select Document
+Step Description: Choose a rendered document to apply password protection.
+Expected Result: The API accepts the document selection request and acknowledges the document to be protected.
+Set Password
+Step Description: Send a request to set a password for the selected document.
+Expected Result: The API accepts the password and confirms its successful assignment to the document.
+Apply Password Protection
+Step Description: Trigger the API to apply password protection to the document using the provided password.
+Expected Result: The API processes the document and returns a success response indicating that password protection has been applied.
+Send Document to Client via Adapter
+Step Description: Use the adapter to send the password-protected document to the client.
+Expected Result: The adapter successfully communicates with the API, retrieves the protected document, and forwards it to the designated client.
+Client Receives Document
+Step Description: Verify that the client receives the password-protected document via the adapter.
+Expected Result: The client application or system should receive the document without any loss of data or corruption.
+Attempt to Open Document without Password
+Step Description: Instruct the client to attempt to open the received document without providing any password.
+Expected Result: Access to the document should be denied, and the client should be prompted to enter a password.
+Attempt to Open Document with Incorrect Password
+Step Description: Instruct the client to attempt to open the document with an incorrect password.
+Expected Result: Access to the document should be denied, and the client should receive an error indicating an incorrect password.
+Open Document with Correct Password
+Step Description: Instruct the client to open the document using the correct password.
+Expected Result: Access to the document should be granted, and the document contents should be visible and intact.</t>
+  </si>
+  <si>
+    <t>The document remains securely password-protected until accessed by the client with the correct password.
+The adapter should log any communication errors or exceptions for troubleshooting purposes.</t>
+  </si>
+  <si>
+    <t>Ensure that the adapter securely communicates with both the API and the client, using appropriate encryption and authentication mechanisms.
+Test the adapter's ability to handle concurrent requests and large document sizes to ensure scalability and performance.
+Consider implementing timeout mechanisms to handle cases where document retrieval or transmission takes longer than expected.</t>
+  </si>
+  <si>
+    <t>Verify Writing Status of Message to DSMQ</t>
+  </si>
+  <si>
+    <t>Ensure that the API successfully writes the status of a message to the DSMQ.</t>
+  </si>
+  <si>
+    <t>Access to the API under test.
+Access to the DSMQ where the message status will be written.
+Message or request ID for testing.</t>
+  </si>
+  <si>
+    <t>Authenticate with API
+Step Description: Authenticate with the API using valid credentials (e.g., API key, OAuth token).
+Expected Result: Successful authentication response with a valid token or session established.
+Prepare Message Status Data
+Step Description: Prepare the data containing the status of the message to be written to the DSMQ. This data should include:
+Message ID or Request ID.
+Status of the message (e.g., "Processing", "Completed", "Failed").
+Additional metadata relevant to the message status (optional).
+Expected Result: Message status data is properly formatted and ready for writing to the DSMQ.
+Write Status of Message to DSMQ
+Step Description: Send a request to the API to write the status of the message to the DSMQ, providing the prepared message status data.
+Expected Result: The API successfully writes the message status data to the DSMQ and returns a success response indicating that the operation was completed.
+Verify Status Data in DSMQ
+Step Description: Access the DSMQ where the message status was written and verify that the status data is present and correctly formatted.
+Expected Result: The status data for the message should be visible in the DSMQ and should match the data sent in the API request.
+Check for Error Handling
+Step Description: Send a request to the API to write the status of a non-existent message or with invalid data.
+Expected Result: The API should handle the error gracefully and return an appropriate error response indicating the reason for failure (e.g., invalid message ID, missing status data).</t>
+  </si>
+  <si>
+    <t>The status of the message is recorded in the DSMQ for further processing or tracking.
+Any error or exception messages should be logged for troubleshooting purposes.</t>
+  </si>
+  <si>
+    <t>Ensure that the API request includes proper error handling mechanisms to deal with communication failures or DSMQ unavailability.
+Consider implementing retries or fallback mechanisms in case of temporary DSMQ outages to ensure data integrity.
+Test the performance of the API when writing status data to the DSMQ under different load conditions to ensure scalability and reliability.</t>
   </si>
 </sst>
 </file>
@@ -2331,15 +2787,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2358,7 +2805,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2663,20 +3121,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3096,20 +3554,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3448,18 +3906,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -4760,18 +5218,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>383</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -5157,28 +5615,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2630F56D-01BC-468E-A632-55FBB048E4ED}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -5212,14 +5670,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="23" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:10" s="20" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>491</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="18" t="s">
         <v>123</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -5244,11 +5702,11 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="20" customFormat="1" ht="245.4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="17" customFormat="1" ht="245.4" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>492</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -5274,11 +5732,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="20" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" s="17" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>493</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5306,64 +5764,354 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:10" s="22" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
         <v>494</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="19" t="s">
         <v>496</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="26" t="s">
         <v>494</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="26" t="s">
         <v>495</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="26" t="s">
         <v>497</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="21" t="s">
         <v>500</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="26" t="s">
         <v>498</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="26" t="s">
         <v>499</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="I6" s="21"/>
+      <c r="J6" s="26" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" s="26" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" s="22" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>502</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>507</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>508</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>509</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>510</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="26" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="22" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>514</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="26" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="22" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>520</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>505</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>521</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>522</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>524</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>525</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>526</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="26" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="22" customFormat="1" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>528</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>529</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>531</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>532</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>533</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>535</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>534</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="26" t="s">
+        <v>537</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="22" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>538</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>539</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>540</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>541</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>543</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>545</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>542</v>
+      </c>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>546</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>547</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>550</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>553</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="26" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>556</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>548</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>557</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>561</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>562</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>549</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="G14" s="26"/>
+      <c r="H14" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>569</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>573</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="8" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>578</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>579</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>584</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>585</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8" t="s">
+        <v>588</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="8" t="s">
+        <v>589</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added few test cases
</commit_message>
<xml_diff>
--- a/surendra_testCases.xlsx
+++ b/surendra_testCases.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepoDATA\CMA_Project\New_Project_CMA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000A0F77-2770-4A90-9029-93AB1062BF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario1" sheetId="1" r:id="rId1"/>
@@ -17,8 +23,8 @@
     <sheet name="flow notes" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="971">
   <si>
     <t>Email with only a subject and a Body Rendered in DocFusion</t>
   </si>
@@ -3778,12 +3784,293 @@
 Email API endpoint URL.
 Database connection details for Message Components Database.</t>
   </si>
+  <si>
+    <t>The Email Doc Gen service is up and running.
+The message components DB is accessible.</t>
+  </si>
+  <si>
+    <t>Trigger an event that would normally cause Email Doc Gen to generate an email. This could involve simulating an email notification or using a tool to interact with the Event Queue Layer.
+Verify that a new message record is created in the message components DB. You can do this by querying the DB directly or using a database management tool.
+Validate the message content in the DB to ensure it matches the expected content of the email that should have been generated. This may involve checking fields such as recipient email address, subject line, and body content.</t>
+  </si>
+  <si>
+    <t>A new message record is created in the message components DB.
+The message content in the DB matches the expected content of the email that should have been generated.</t>
+  </si>
+  <si>
+    <t>Pass: The test case passes if a new message record is created in the message components DB with the expected content.
+Fail: The test case fails if no new message record is created in the message components DB, or if the message content does not match the expected content.</t>
+  </si>
+  <si>
+    <t>The Email Password Protect functionality is enabled.
+The message components DB is accessible.</t>
+  </si>
+  <si>
+    <t>Send an email that requires password protection. This might involve using a specific feature within the system or manually adding a password protection flag.
+Verify that a new message record is created in the message components DB. You can do this by querying the DB directly or using a database management tool.
+Validate the message content in the DB to ensure it includes a password field or reference to password protection.</t>
+  </si>
+  <si>
+    <t>A new message record is created in the message components DB.
+The message content includes a password field or a flag indicating password protection is applied.</t>
+  </si>
+  <si>
+    <t>Pass: The test case passes if a new message record is created in the message components DB with a password field or reference to password protection.
+Fail: The test case fails if no new message record is created in the message components DB, or if there's no indication of password protection within the message content.</t>
+  </si>
+  <si>
+    <t>The Email Orchestrator service is up and running.
+The message components DB is accessible.</t>
+  </si>
+  <si>
+    <t>Trigger an event that would normally cause the Email Orchestrator to send an email. This could involve simulating an email notification or using a tool to interact with the Email Orchestrator service.
+Verify that a new message record is created in the message components DB. You can do this by querying the DB directly or using a database management tool.
+Validate the message content in the DB to ensure it matches the expected content of the email that should have been orchestrated. This may involve checking fields such as recipient email address, subject line, and body content.</t>
+  </si>
+  <si>
+    <t>A new message record is created in the message components DB.
+The message content in the DB matches the expected content of the email that should have been orchestrated.</t>
+  </si>
+  <si>
+    <t>The Email DocGen service is up and running.
+The message components DB is accessible.</t>
+  </si>
+  <si>
+    <t>Trigger an event that would normally cause Email DocGen to generate an email document. This could involve:
+Simulating an action that triggers a notification email (e.g., user registration).
+Using a testing tool to interact with the system and initiate the document generation process.
+Verify that a new message record is created in the message components DB. You can achieve this by:
+Querying the DB directly using a SQL query tool.
+Using a database management tool to view recently added records.
+Validate the message content in the DB to ensure it matches the expected email content. This may involve checking fields such as:
+Recipient email address (if applicable).
+Subject line.
+Body content containing the generated document information.
+Any additional fields specific to DocGen messages (e.g., document type, template used).</t>
+  </si>
+  <si>
+    <t>Pass: The test case passes if:
+A new message record exists in the message components DB.
+The message content matches the expected DocGen email content.
+Fail: The test case fails if:
+No new message record is created in the DB.
+The message content does not match the expected DocGen email content.</t>
+  </si>
+  <si>
+    <t>A new message record is created in the message components DB.
+The message content matches the expected content of the email that should have been generated by Email DocGen.You can delete the test message record from the DB after the test is complete.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depending on your Email DocGen implementation, you might need to prepare specific data to trigger the document generation </t>
+  </si>
+  <si>
+    <t>The Email functionality with password protection is enabled.
+The message components DB is accessible.</t>
+  </si>
+  <si>
+    <t>Send an email requiring password protection. This might involve:
+Using a dedicated "password protect" feature within the system.
+Manually adding a password protection flag during email creation (if supported).
+Verify that a new message record is created in the message components DB. You can achieve this by:
+Querying the DB directly with a SQL query targeting recently added records.
+Using a database management tool to view new entries.
+Validate the message content in the DB to ensure it includes password information. This may involve checking for:
+A dedicated field storing the password itself (caution: avoid storing actual passwords in test data).
+A flag indicating password protection is applied.
+An encrypted representation of the password (depending on the implementation)</t>
+  </si>
+  <si>
+    <t>A new message record is created in the message components DB.
+The message content includes a field or reference indicating password protection is applied.</t>
+  </si>
+  <si>
+    <t>Pass: The test case passes if:
+A new message record exists in the message components DB.
+The message content includes a field or reference indicating password protection.You can delete the test message record from the DB after the test is complete.
+Fail: The test case fails if:
+No new message record is created in the DB.
+There's no indication of password protection within the message content.</t>
+  </si>
+  <si>
+    <t>An email with password protection enabled</t>
+  </si>
+  <si>
+    <t>The primary message processing system is unavailable (simulated or actual failover).
+The Failover Topic exists and is configured correctly.
+The Inegestion Queue for the Email Topic exists and is accessible.</t>
+  </si>
+  <si>
+    <t>Simulate a failover event:
+Stop the primary message processing system (if a simulated failover).
+Alternatively, induce a failover event using your system's specific failover mechanism.
+Trigger an event that would normally be processed by the primary system and generate a message.
+Verify message presence in the Failover Topic:
+Use a message broker monitoring tool to confirm the message arrived in the Failover Topic.
+Alternatively, query the Failover Topic directly using a dedicated client (if supported).
+Simulate failover recovery (optional):
+Restart the primary message processing system (if a simulated failover).
+Allow the system to recover from the failover event naturally.
+Verify message presence in the Inegestion Queue for the Email Topic:
+Use a queue monitoring tool to confirm the message was routed to the Inegestion Queue.
+Alternatively, query the Inegestion Queue directly using a dedicated client (if supported).</t>
+  </si>
+  <si>
+    <t>The message is published to the Failover Topic during the failover event.
+After failover recovery (or simulated recovery), the message is present in the Inegestion Queue for the Email Topic.</t>
+  </si>
+  <si>
+    <t>Pass: The test case passes if:
+The message is published to the Failover Topic during the failover event.
+The message is present in the Inegestion Queue for the Email Topic after failover recovery.
+Fail: The test case fails if:
+The message is not published to the Failover Topic.
+The message is not present in the Inegestion Queue for the Email Topic after failover recovery.</t>
+  </si>
+  <si>
+    <t>The Email Orchestrator system should be up and running.
+Ingestion Queue is operational and able to receive messages.
+Necessary API endpoints are accessible.</t>
+  </si>
+  <si>
+    <t>Prepare an email message that exceeds the maximum size limit supported by the Email Orchestrator.
+Use the test data provided above and ensure the body text is large enough to trigger the breaking functionality.
+Send the prepared email message to the Ingestion Queue.
+Use a tool or script to push the email message into the Ingestion Queue.
+Monitor the Ingestion Queue to ensure the message is received.
+Verify the email message appears in the Ingestion Queue.
+Verify the Email Orchestrator picks up the email message from the Ingestion Queue.
+Check the processing logs of the Email Orchestrator.
+Verify that the Email Orchestrator breaks the email message into multiple parts.
+Ensure each part is within the maximum size limit and properly formatted.
+Confirm that all broken parts are queued in the Adapter Queue.
+Check the Adapter Queue to see if all parts of the original message are present.
+Verify each part is sent through the appropriate channels (e.g., SMTP, SendGrid).
+Check the logs or monitoring tools to ensure each part is processed and sent correctly.
+Validate the complete email is received by the recipient.
+Send the broken parts to a test email account and verify the email can be reassembled correctly.</t>
+  </si>
+  <si>
+    <t>The email message should be broken into multiple parts if it exceeds the maximum size limit.
+Each part should be correctly formatted and within the size limit.
+All parts should be queued in the Adapter Queue and processed by the appropriate channels.
+The recipient should receive the email, and it should be reassembled correctly, maintaining the original content.</t>
+  </si>
+  <si>
+    <t>The system should clear the test email from the queues.
+Logs should be reviewed and maintained for future reference.</t>
+  </si>
+  <si>
+    <t>The Email Orchestrator system should be up and running.
+Ingestion Queue is operational and able to receive messages.
+Necessary API endpoints are accessible.
+SMTP adapters configured and operational.</t>
+  </si>
+  <si>
+    <t>1 Prepare a standard email message.
+Use the test data provided above.
+2 Send the prepared email message to the Ingestion Queue.
+Use a tool or script to push the email message into the Ingestion Queue.
+3 Monitor the Ingestion Queue to ensure the message is received.
+Verify the email message appears in the Ingestion Queue.
+4 Verify the Email Orchestrator picks up the email message from the Ingestion Queue.
+Check the processing logs of the Email Orchestrator.
+5 Verify the Email Orchestrator processes the email through the Email Completion module.
+Ensure the email goes through the necessary steps of the Email Completion process.
+6 Check if the email is placed in the Adapter Queue after completion.
+Ensure the processed email appears in the Adapter Queue.
+7 Confirm that the email in the Adapter Queue is directed to the SMTP adapters.
+Check the Adapter Queue to see if the email is being routed to the SMTP adapters.
+8 Verify that the email is sent through the SMTP adapters.
+Use logs or monitoring tools to confirm the email is handed over to the SMTP adapters.
+9 Validate the email is successfully received by the recipient.
+Send the email to a test email account and verify its receipt.</t>
+  </si>
+  <si>
+    <t>The email message should be processed through the Email Completion module without errors.
+The completed email should be queued in the Adapter Queue.
+The email should be correctly routed to the SMTP adapters from the Adapter Queue.
+The recipient should receive the email successfully through the SMTP channel.</t>
+  </si>
+  <si>
+    <t>The Email Orchestrator system should be up and running.
+Ingestion Queue is operational and able to receive messages.
+Necessary API endpoints are accessible.
+SendGrid adapters configured and operational.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 Prepare a standard email message.
+Use the test data provided above.
+ 2 Send the prepared email message to the Ingestion Queue.
+Use a tool or script to push the email message into the Ingestion Queue.
+ 3 Monitor the Ingestion Queue to ensure the message is received.
+Verify the email message appears in the Ingestion Queue.
+ 4 Verify the Email Orchestrator picks up the email message from the Ingestion Queue.
+Check the processing logs of the Email Orchestrator.
+ 5 Verify the Email Orchestrator processes the email through the Email Completion module.
+Ensure the email goes through the necessary s of the Email Completion process.
+ 6 Check if the email is placed in the Adapter Queue after completion.
+Ensure the processed email appears in the Adapter Queue.
+ 7 Confirm that the email in the Adapter Queue is directed to the SendGrid adapters.
+Check the Adapter Queue to see if the email is being routed to the SendGrid adapters.
+ 8 Verify that the email is sent through the SendGrid adapters.
+Use logs or monitoring tools to confirm the email is handed over to the SendGrid adapters.
+ 9 Validate the email is successfully received by the recipient.
+Send the email to a test email account and verify its receipt.</t>
+  </si>
+  <si>
+    <t>The email message should be processed through the Email Completion module without errors.
+The completed email should be queued in the Adapter Queue.
+The email should be correctly routed to the SendGrid adapters from the Adapter Queue.The recipient should receive the email successfully through the SendGrid channel.</t>
+  </si>
+  <si>
+    <t>The Email Orchestrator system should be up and running.
+Ingestion Queue is operational and able to receive messages.
+Email Completion module is operational.
+SendGrid adapters configured and operational.
+Necessary API endpoints are accessible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 Prepare a standard email message.
+Use the test data provided above.
+ 2 Send the prepared email message to the Ingestion Queue.
+Use a tool or script to push the email message into the Ingestion Queue.
+ 3 Monitor the Ingestion Queue to ensure the message is received.
+Verify the email message appears in the Ingestion Queue.
+ 4 Verify the Email Orchestrator picks up the email message from the Ingestion Queue.
+Check the processing logs of the Email Orchestrator.
+ 5 Verify the Email Orchestrator processes the email through the Email Completion module.
+Ensure the email goes through the necessary s of the Email Completion process.
+ 6 Check if the email is placed in the Adapter Queue after completion.
+Ensure the processed email appears in the Adapter Queue.
+ 7 Confirm that the email in the Adapter Queue is directed to the SendGrid adapters.
+Check the Adapter Queue to see if the email is being routed to the SendGrid adapters.
+ 8 Verify that the SendGrid adapters pick up the email from the Adapter Queue.
+Use logs or monitoring tools to confirm the email is handed over to the SendGrid adapters.
+ 9 Validate the email is successfully sent by the SendGrid adapters.
+Check the SendGrid adapter logs or dashboard to ensure the email is processed and sent.
+ 10 Validate the email is successfully received by the recipient.
+Send the email to a test email account and verify its receipt.</t>
+  </si>
+  <si>
+    <t>The email message should be processed through the Email Completion module without errors.
+The completed email should be queued in the Adapter Queue.
+The email should be correctly routed to the SendGrid adapters from the Adapter Queue.
+The SendGrid adapters should pick up the email and process it.
+The recipient should receive the email successfully through the SendGrid channel.</t>
+  </si>
+  <si>
+    <t>The Email Orchestrator system should be up and running.
+Ingestion Queue is operational and able to receive messages.
+Failover Engine is operational.
+Necessary API endpoints are accessible.
+Failover mechanisms configured.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4331,14 +4618,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
@@ -4347,22 +4634,22 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="42" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="40.42578125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="35.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="40.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -4378,7 +4665,7 @@
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -4412,7 +4699,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="225">
+    <row r="3" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -4446,7 +4733,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="195">
+    <row r="4" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -4478,7 +4765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="240">
+    <row r="5" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -4510,7 +4797,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="270">
+    <row r="6" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
@@ -4542,7 +4829,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="255">
+    <row r="7" spans="1:12" ht="216" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
@@ -4574,7 +4861,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="225">
+    <row r="8" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -4606,7 +4893,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="255">
+    <row r="9" spans="1:12" ht="244.8" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>70</v>
       </c>
@@ -4638,7 +4925,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="240">
+    <row r="10" spans="1:12" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
@@ -4670,7 +4957,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="405">
+    <row r="11" spans="1:12" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>90</v>
       </c>
@@ -4702,7 +4989,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="285">
+    <row r="12" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>100</v>
       </c>
@@ -4734,7 +5021,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="285">
+    <row r="13" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>110</v>
       </c>
@@ -4776,7 +5063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView zoomScale="58" workbookViewId="0">
@@ -4785,17 +5072,17 @@
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="40.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" style="7"/>
-    <col min="2" max="2" width="16.85546875" style="7" customWidth="1"/>
-    <col min="3" max="7" width="40.28515625" style="7"/>
-    <col min="8" max="8" width="40.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="40.28515625" style="7"/>
+    <col min="1" max="1" width="40.33203125" style="7"/>
+    <col min="2" max="2" width="16.88671875" style="7" customWidth="1"/>
+    <col min="3" max="7" width="40.33203125" style="7"/>
+    <col min="8" max="8" width="40.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="40.33203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>120</v>
       </c>
@@ -4811,7 +5098,7 @@
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1">
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -4843,7 +5130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="179.45" customHeight="1">
+    <row r="3" spans="1:12" ht="179.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>121</v>
       </c>
@@ -4875,7 +5162,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="315">
+    <row r="4" spans="1:12" ht="288.60000000000002" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>130</v>
       </c>
@@ -4904,7 +5191,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="270">
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -4936,7 +5223,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" ht="225">
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>50</v>
       </c>
@@ -4968,7 +5255,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" ht="240">
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="216" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>70</v>
       </c>
@@ -5000,7 +5287,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="210">
+    <row r="8" spans="1:12" ht="202.2" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>141</v>
       </c>
@@ -5029,7 +5316,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="210">
+    <row r="9" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>149</v>
       </c>
@@ -5058,7 +5345,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="285">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>100</v>
       </c>
@@ -5090,7 +5377,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="315">
+    <row r="11" spans="1:12" s="1" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>110</v>
       </c>
@@ -5132,7 +5419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5140,14 +5427,14 @@
       <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="34.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="34.85546875" style="9"/>
-    <col min="6" max="6" width="14.28515625" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="34.85546875" style="9"/>
+    <col min="1" max="5" width="34.88671875" style="9"/>
+    <col min="6" max="6" width="14.33203125" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="34.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>159</v>
       </c>
@@ -5161,7 +5448,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:10" ht="30">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -5193,7 +5480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="105">
+    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>160</v>
       </c>
@@ -5217,7 +5504,7 @@
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="90">
+    <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>165</v>
       </c>
@@ -5241,7 +5528,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="105">
+    <row r="5" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>170</v>
       </c>
@@ -5265,7 +5552,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="90">
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>174</v>
       </c>
@@ -5289,7 +5576,7 @@
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="90">
+    <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>179</v>
       </c>
@@ -5313,7 +5600,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="75">
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>184</v>
       </c>
@@ -5337,7 +5624,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="120">
+    <row r="9" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>189</v>
       </c>
@@ -5361,7 +5648,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" ht="105">
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>193</v>
       </c>
@@ -5385,7 +5672,7 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" ht="105">
+    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>197</v>
       </c>
@@ -5409,7 +5696,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="105">
+    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>201</v>
       </c>
@@ -5433,7 +5720,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="105">
+    <row r="13" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>205</v>
       </c>
@@ -5457,7 +5744,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="60">
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>209</v>
       </c>
@@ -5481,7 +5768,7 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="60">
+    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>179</v>
       </c>
@@ -5505,7 +5792,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="60">
+    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>217</v>
       </c>
@@ -5529,7 +5816,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" ht="60">
+    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>221</v>
       </c>
@@ -5553,7 +5840,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="75">
+    <row r="18" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>226</v>
       </c>
@@ -5577,7 +5864,7 @@
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:10" ht="75">
+    <row r="19" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>230</v>
       </c>
@@ -5601,7 +5888,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" spans="1:10" ht="75">
+    <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>235</v>
       </c>
@@ -5625,7 +5912,7 @@
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
     </row>
-    <row r="21" spans="1:10" ht="75">
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>239</v>
       </c>
@@ -5649,7 +5936,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="75">
+    <row r="22" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>243</v>
       </c>
@@ -5673,7 +5960,7 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10" ht="75">
+    <row r="23" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>248</v>
       </c>
@@ -5697,7 +5984,7 @@
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:10" ht="75">
+    <row r="24" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>252</v>
       </c>
@@ -5721,7 +6008,7 @@
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="1:10" ht="90">
+    <row r="25" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>256</v>
       </c>
@@ -5745,7 +6032,7 @@
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:10" ht="105">
+    <row r="26" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>261</v>
       </c>
@@ -5769,7 +6056,7 @@
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="1:10" ht="105">
+    <row r="27" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>265</v>
       </c>
@@ -5793,7 +6080,7 @@
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="1:10" ht="60">
+    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>271</v>
       </c>
@@ -5817,7 +6104,7 @@
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" ht="90">
+    <row r="29" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>276</v>
       </c>
@@ -5841,7 +6128,7 @@
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
     </row>
-    <row r="30" spans="1:10" ht="90">
+    <row r="30" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>281</v>
       </c>
@@ -5865,7 +6152,7 @@
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
     </row>
-    <row r="31" spans="1:10" ht="75">
+    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>286</v>
       </c>
@@ -5889,7 +6176,7 @@
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
     </row>
-    <row r="32" spans="1:10" ht="75">
+    <row r="32" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>290</v>
       </c>
@@ -5913,7 +6200,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" ht="60">
+    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>295</v>
       </c>
@@ -5937,7 +6224,7 @@
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:10" ht="75">
+    <row r="34" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>299</v>
       </c>
@@ -5961,7 +6248,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" ht="60">
+    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>303</v>
       </c>
@@ -5985,7 +6272,7 @@
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
     </row>
-    <row r="36" spans="1:10" ht="60">
+    <row r="36" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>307</v>
       </c>
@@ -6009,7 +6296,7 @@
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
     </row>
-    <row r="37" spans="1:10" ht="75">
+    <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>311</v>
       </c>
@@ -6033,7 +6320,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="1:10" ht="75">
+    <row r="38" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>316</v>
       </c>
@@ -6057,7 +6344,7 @@
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="1:10" ht="409.5">
+    <row r="39" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>80</v>
       </c>
@@ -6089,7 +6376,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="90">
+    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>322</v>
       </c>
@@ -6113,7 +6400,7 @@
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="1:10" ht="90">
+    <row r="41" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>327</v>
       </c>
@@ -6137,7 +6424,7 @@
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:10" ht="120">
+    <row r="42" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>331</v>
       </c>
@@ -6161,7 +6448,7 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="90">
+    <row r="43" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>335</v>
       </c>
@@ -6185,7 +6472,7 @@
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:10" ht="90">
+    <row r="44" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>340</v>
       </c>
@@ -6209,7 +6496,7 @@
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="105">
+    <row r="45" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>345</v>
       </c>
@@ -6233,7 +6520,7 @@
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="1:10" ht="105">
+    <row r="46" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>350</v>
       </c>
@@ -6257,7 +6544,7 @@
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="1:10" ht="90">
+    <row r="47" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>355</v>
       </c>
@@ -6281,7 +6568,7 @@
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="1:10" ht="105">
+    <row r="48" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>360</v>
       </c>
@@ -6305,7 +6592,7 @@
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="1:10" ht="90">
+    <row r="49" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>364</v>
       </c>
@@ -6329,7 +6616,7 @@
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="1:10" ht="120">
+    <row r="50" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>369</v>
       </c>
@@ -6353,7 +6640,7 @@
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
     </row>
-    <row r="51" spans="1:10" ht="105">
+    <row r="51" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>373</v>
       </c>
@@ -6377,7 +6664,7 @@
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
     </row>
-    <row r="52" spans="1:10" ht="105">
+    <row r="52" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>377</v>
       </c>
@@ -6401,7 +6688,7 @@
       <c r="I52" s="10"/>
       <c r="J52" s="10"/>
     </row>
-    <row r="53" spans="1:10" ht="409.5">
+    <row r="53" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>110</v>
       </c>
@@ -6442,7 +6729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -6450,16 +6737,16 @@
       <selection pane="bottomLeft" sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="46.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="46.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.140625" style="9"/>
-    <col min="2" max="2" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="46.140625" style="9"/>
-    <col min="10" max="10" width="6.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="46.140625" style="9"/>
+    <col min="1" max="1" width="46.109375" style="9"/>
+    <col min="2" max="2" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="46.109375" style="9"/>
+    <col min="10" max="10" width="6.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="46.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>383</v>
       </c>
@@ -6473,7 +6760,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -6505,7 +6792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="135">
+    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>384</v>
       </c>
@@ -6531,7 +6818,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="345">
+    <row r="4" spans="1:10" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>392</v>
       </c>
@@ -6558,7 +6845,7 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:10" ht="120">
+    <row r="5" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>400</v>
       </c>
@@ -6584,7 +6871,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="105">
+    <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>408</v>
       </c>
@@ -6610,7 +6897,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="120">
+    <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>416</v>
       </c>
@@ -6636,7 +6923,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="135">
+    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>424</v>
       </c>
@@ -6665,7 +6952,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="120">
+    <row r="9" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>433</v>
       </c>
@@ -6691,7 +6978,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="150">
+    <row r="10" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>441</v>
       </c>
@@ -6717,7 +7004,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="150">
+    <row r="11" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>449</v>
       </c>
@@ -6743,7 +7030,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="180">
+    <row r="12" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>457</v>
       </c>
@@ -6769,7 +7056,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="150">
+    <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>465</v>
       </c>
@@ -6795,7 +7082,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="135">
+    <row r="14" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>473</v>
       </c>
@@ -6821,7 +7108,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="180">
+    <row r="15" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>480</v>
       </c>
@@ -6856,7 +7143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -6864,9 +7151,9 @@
       <selection pane="bottomLeft" sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="47.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="47.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>488</v>
       </c>
@@ -6880,7 +7167,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -6912,7 +7199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="20" customFormat="1" ht="150">
+    <row r="3" spans="1:10" s="20" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>121</v>
       </c>
@@ -6944,7 +7231,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="17" customFormat="1" ht="285">
+    <row r="4" spans="1:10" s="17" customFormat="1" ht="245.4" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>130</v>
       </c>
@@ -6974,7 +7261,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="17" customFormat="1" ht="195">
+    <row r="5" spans="1:10" s="17" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -7006,7 +7293,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="22" customFormat="1" ht="409.5">
+    <row r="6" spans="1:10" s="22" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>494</v>
       </c>
@@ -7036,7 +7323,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="22" customFormat="1" ht="75">
+    <row r="7" spans="1:10" s="22" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>502</v>
       </c>
@@ -7064,7 +7351,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="22" customFormat="1" ht="105">
+    <row r="8" spans="1:10" s="22" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>512</v>
       </c>
@@ -7094,7 +7381,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="22" customFormat="1" ht="180">
+    <row r="9" spans="1:10" s="22" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>520</v>
       </c>
@@ -7124,7 +7411,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="22" customFormat="1" ht="330">
+    <row r="10" spans="1:10" s="22" customFormat="1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>528</v>
       </c>
@@ -7154,7 +7441,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="22" customFormat="1" ht="105">
+    <row r="11" spans="1:10" s="22" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>538</v>
       </c>
@@ -7184,7 +7471,7 @@
       </c>
       <c r="J11" s="21"/>
     </row>
-    <row r="12" spans="1:10" ht="150">
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>546</v>
       </c>
@@ -7214,7 +7501,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="105">
+    <row r="13" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>556</v>
       </c>
@@ -7242,7 +7529,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="409.5">
+    <row r="14" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>562</v>
       </c>
@@ -7270,7 +7557,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="409.5">
+    <row r="15" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>569</v>
       </c>
@@ -7296,7 +7583,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="409.5">
+    <row r="16" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>578</v>
       </c>
@@ -7322,7 +7609,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="409.5">
+    <row r="17" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>584</v>
       </c>
@@ -7359,7 +7646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -7367,9 +7654,9 @@
       <selection pane="bottomLeft" sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="29.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>590</v>
       </c>
@@ -7383,7 +7670,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -7415,7 +7702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="25" customFormat="1" ht="60">
+    <row r="3" spans="1:10" s="25" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>618</v>
       </c>
@@ -7439,7 +7726,7 @@
       <c r="I3" s="26"/>
       <c r="J3" s="26"/>
     </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" ht="60">
+    <row r="4" spans="1:10" s="25" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>617</v>
       </c>
@@ -7463,7 +7750,7 @@
       <c r="I4" s="26"/>
       <c r="J4" s="26"/>
     </row>
-    <row r="5" spans="1:10" s="25" customFormat="1" ht="75">
+    <row r="5" spans="1:10" s="25" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>616</v>
       </c>
@@ -7487,7 +7774,7 @@
       <c r="I5" s="26"/>
       <c r="J5" s="26"/>
     </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" ht="75">
+    <row r="6" spans="1:10" s="25" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>615</v>
       </c>
@@ -7511,7 +7798,7 @@
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" ht="75">
+    <row r="7" spans="1:10" s="25" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>619</v>
       </c>
@@ -7535,7 +7822,7 @@
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
     </row>
-    <row r="8" spans="1:10" s="25" customFormat="1" ht="105">
+    <row r="8" spans="1:10" s="25" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>624</v>
       </c>
@@ -7559,7 +7846,7 @@
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
     </row>
-    <row r="9" spans="1:10" s="25" customFormat="1" ht="105">
+    <row r="9" spans="1:10" s="25" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>629</v>
       </c>
@@ -7583,7 +7870,7 @@
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
     </row>
-    <row r="10" spans="1:10" s="25" customFormat="1" ht="120">
+    <row r="10" spans="1:10" s="25" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>634</v>
       </c>
@@ -7607,7 +7894,7 @@
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" spans="1:10" s="25" customFormat="1" ht="75">
+    <row r="11" spans="1:10" s="25" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>639</v>
       </c>
@@ -7631,7 +7918,7 @@
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="1:10" s="25" customFormat="1" ht="90">
+    <row r="12" spans="1:10" s="25" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>644</v>
       </c>
@@ -7655,7 +7942,7 @@
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
     </row>
-    <row r="13" spans="1:10" s="25" customFormat="1" ht="45">
+    <row r="13" spans="1:10" s="25" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>652</v>
       </c>
@@ -7679,7 +7966,7 @@
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
     </row>
-    <row r="14" spans="1:10" s="25" customFormat="1" ht="45">
+    <row r="14" spans="1:10" s="25" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>660</v>
       </c>
@@ -7703,7 +7990,7 @@
       <c r="I14" s="26"/>
       <c r="J14" s="26"/>
     </row>
-    <row r="15" spans="1:10" s="25" customFormat="1" ht="45">
+    <row r="15" spans="1:10" s="25" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>665</v>
       </c>
@@ -7727,7 +8014,7 @@
       <c r="I15" s="26"/>
       <c r="J15" s="26"/>
     </row>
-    <row r="16" spans="1:10" s="25" customFormat="1" ht="120">
+    <row r="16" spans="1:10" s="25" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>670</v>
       </c>
@@ -7751,7 +8038,7 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
     </row>
-    <row r="17" spans="1:10" s="25" customFormat="1" ht="105">
+    <row r="17" spans="1:10" s="25" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>675</v>
       </c>
@@ -7775,7 +8062,7 @@
       <c r="I17" s="26"/>
       <c r="J17" s="26"/>
     </row>
-    <row r="18" spans="1:10" s="25" customFormat="1">
+    <row r="18" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24"/>
       <c r="B18" s="27"/>
       <c r="C18" s="24"/>
@@ -7787,7 +8074,7 @@
       <c r="I18" s="24"/>
       <c r="J18" s="24"/>
     </row>
-    <row r="19" spans="1:10" s="25" customFormat="1">
+    <row r="19" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
       <c r="B19" s="26"/>
       <c r="C19" s="24"/>
@@ -7799,7 +8086,7 @@
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
     </row>
-    <row r="20" spans="1:10" s="25" customFormat="1">
+    <row r="20" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
       <c r="B20" s="26"/>
       <c r="C20" s="24"/>
@@ -7811,7 +8098,7 @@
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -7833,7 +8120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7842,19 +8129,19 @@
       <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5546875" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>677</v>
       </c>
@@ -7868,7 +8155,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -7900,7 +8187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>678</v>
       </c>
@@ -7924,7 +8211,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="45">
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>684</v>
       </c>
@@ -7948,7 +8235,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="45">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>695</v>
       </c>
@@ -7972,7 +8259,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="60">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>699</v>
       </c>
@@ -7996,7 +8283,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="60">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>705</v>
       </c>
@@ -8020,7 +8307,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="60" hidden="1">
+    <row r="8" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>709</v>
       </c>
@@ -8044,7 +8331,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="60" hidden="1">
+    <row r="9" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>713</v>
       </c>
@@ -8068,7 +8355,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="60">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>721</v>
       </c>
@@ -8092,7 +8379,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="60">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>725</v>
       </c>
@@ -8116,7 +8403,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="60">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>616</v>
       </c>
@@ -8140,7 +8427,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="45" hidden="1">
+    <row r="13" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>735</v>
       </c>
@@ -8164,7 +8451,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="45" hidden="1">
+    <row r="14" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>748</v>
       </c>
@@ -8188,7 +8475,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="45" hidden="1">
+    <row r="15" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>752</v>
       </c>
@@ -8212,7 +8499,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" ht="45" hidden="1">
+    <row r="16" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>756</v>
       </c>
@@ -8234,7 +8521,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="60" hidden="1">
+    <row r="17" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>761</v>
       </c>
@@ -8258,7 +8545,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="45">
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>765</v>
       </c>
@@ -8282,7 +8569,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" ht="60">
+    <row r="19" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>770</v>
       </c>
@@ -8306,7 +8593,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" ht="75" hidden="1">
+    <row r="20" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>775</v>
       </c>
@@ -8330,7 +8617,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:10" ht="60">
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>778</v>
       </c>
@@ -8354,7 +8641,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" ht="60">
+    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>782</v>
       </c>
@@ -8378,7 +8665,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:10" ht="60">
+    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>789</v>
       </c>
@@ -8402,7 +8689,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" ht="90">
+    <row r="24" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>797</v>
       </c>
@@ -8426,7 +8713,7 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" ht="90">
+    <row r="25" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>802</v>
       </c>
@@ -8450,7 +8737,7 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:10" ht="30">
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>806</v>
       </c>
@@ -8474,7 +8761,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:10" ht="60">
+    <row r="27" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>811</v>
       </c>
@@ -8498,7 +8785,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:10" ht="45">
+    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>819</v>
       </c>
@@ -8522,7 +8809,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10" ht="45">
+    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>824</v>
       </c>
@@ -8546,7 +8833,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" ht="60">
+    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>829</v>
       </c>
@@ -8570,7 +8857,7 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:10" ht="45">
+    <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>836</v>
       </c>
@@ -8594,7 +8881,7 @@
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:10" ht="45">
+    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>841</v>
       </c>
@@ -8627,17 +8914,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="63.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8666,7 +8958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>873</v>
       </c>
@@ -8679,7 +8971,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="210">
+    <row r="3" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>846</v>
       </c>
@@ -8706,7 +8998,7 @@
       </c>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="390">
+    <row r="4" spans="1:9" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>847</v>
       </c>
@@ -8731,7 +9023,7 @@
       </c>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="409.5">
+    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>887</v>
       </c>
@@ -8758,7 +9050,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="409.5">
+    <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>888</v>
       </c>
@@ -8783,7 +9075,7 @@
       </c>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" ht="409.5">
+    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>894</v>
       </c>
@@ -8808,7 +9100,7 @@
       </c>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" ht="409.5">
+    <row r="8" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>849</v>
       </c>
@@ -8833,7 +9125,7 @@
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="409.5">
+    <row r="9" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>851</v>
       </c>
@@ -8858,157 +9150,241 @@
       </c>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" ht="45">
+    <row r="10" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>853</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>852</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>932</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>933</v>
+      </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>934</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>935</v>
+      </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" ht="45">
+    <row r="11" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>854</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>852</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>936</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>937</v>
+      </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>938</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>939</v>
+      </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" ht="45">
+    <row r="12" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>868</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>850</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>940</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>941</v>
+      </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>942</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>935</v>
+      </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" ht="45">
+    <row r="13" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>869</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>850</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>943</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>944</v>
+      </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>946</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>945</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>947</v>
+      </c>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" ht="45">
+    <row r="14" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>870</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>850</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>948</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>949</v>
+      </c>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>950</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>951</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>952</v>
+      </c>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="60">
+    <row r="15" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>893</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>850</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>953</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>954</v>
+      </c>
       <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>955</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>956</v>
+      </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" ht="45">
+    <row r="16" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>855</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>852</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>957</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>958</v>
+      </c>
       <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>960</v>
+      </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" ht="30">
+    <row r="17" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>857</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>852</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>962</v>
+      </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>963</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>960</v>
+      </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" ht="30">
+    <row r="18" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>856</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>852</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>964</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>965</v>
+      </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>966</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>960</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" ht="45">
+    <row r="19" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>858</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>859</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>967</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>968</v>
+      </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>969</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>960</v>
+      </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:9" ht="45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>860</v>
       </c>
@@ -9023,14 +9399,16 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" ht="45">
+    <row r="21" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>892</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>859</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="8" t="s">
+        <v>970</v>
+      </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -9038,7 +9416,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:9" ht="60">
+    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>871</v>
       </c>
@@ -9053,7 +9431,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" ht="45">
+    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>872</v>
       </c>
@@ -9068,7 +9446,7 @@
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" ht="150">
+    <row r="24" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>863</v>
       </c>
@@ -9083,7 +9461,7 @@
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:9" ht="150">
+    <row r="25" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>862</v>
       </c>
@@ -9098,7 +9476,7 @@
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" ht="60">
+    <row r="26" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>864</v>
       </c>
@@ -9113,7 +9491,7 @@
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" ht="60">
+    <row r="27" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>866</v>
       </c>
@@ -9128,7 +9506,7 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" ht="30">
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>891</v>
       </c>
@@ -9143,7 +9521,7 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" ht="45">
+    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>867</v>
       </c>
@@ -9158,7 +9536,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -9169,7 +9547,7 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" ht="45">
+    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
         <v>874</v>
       </c>
@@ -9182,7 +9560,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" ht="60">
+    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>875</v>
       </c>
@@ -9197,7 +9575,7 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" ht="60">
+    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>877</v>
       </c>
@@ -9212,7 +9590,7 @@
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" ht="60">
+    <row r="34" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>878</v>
       </c>
@@ -9227,7 +9605,7 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="29" t="s">
         <v>879</v>
       </c>
@@ -9240,7 +9618,7 @@
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" ht="45">
+    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>880</v>
       </c>
@@ -9255,7 +9633,7 @@
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" ht="45">
+    <row r="37" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>882</v>
       </c>
@@ -9270,7 +9648,7 @@
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" ht="60">
+    <row r="38" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>883</v>
       </c>
@@ -9285,7 +9663,7 @@
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" ht="90">
+    <row r="39" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>884</v>
       </c>
@@ -9300,7 +9678,7 @@
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" ht="90">
+    <row r="40" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>885</v>
       </c>
@@ -9315,7 +9693,7 @@
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" ht="30">
+    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>890</v>
       </c>
@@ -9330,7 +9708,7 @@
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -9341,7 +9719,7 @@
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>

</xml_diff>